<commit_message>
Fix Fragen in Auswertungsdaten darstellen
</commit_message>
<xml_diff>
--- a/data/auswertung-freitext-kategorien-open-access-meinung-30815.xlsx
+++ b/data/auswertung-freitext-kategorien-open-access-meinung-30815.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="153">
   <si>
     <t xml:space="preserve"> ich arbeite vorwiegend in präkeren arbeitsverhältnissen und investiere unbezahlte zeit in das verfassen meiner texte. wenn es die möglichkeit gibt, zumindest ein kleines honorar zu bekommen, dann bevorzuge ich das - ich muss ja irgendwie meine miete, mein essen, etc bezahlen.</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>a = Anerkennung, f = finanzielle Aspekte, q= Qualitäts Aspekte, s= strukturelle r=rechtliche, wf = wissenschaftsfreiheit</t>
+  </si>
+  <si>
+    <t>Frage: Bitte kommentieren Sie kurz Ihre Meinung zu der Forderung nach kostenfreiem Zugang zu allen wissenschaftlichen Publikationen (Open Access)</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -783,7 +788,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="245">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -905,6 +910,7 @@
     <cellStyle name="Besuchter Link" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1026,6 +1032,7 @@
     <cellStyle name="Link" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1355,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1366,211 +1373,216 @@
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49" customHeight="1">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="49" customHeight="1">
+      <c r="B2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2">
-        <v>63</v>
-      </c>
-      <c r="C2">
-        <v>32</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>26</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>26</v>
+      </c>
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>21</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>138</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="B5">
-        <f>SUM(B2:B4)</f>
+    <row r="6" spans="1:8">
+      <c r="B6">
+        <f>SUM(B3:B5)</f>
         <v>81</v>
       </c>
-      <c r="C5">
-        <f>SUM(C2:C4)</f>
+      <c r="C6">
+        <f>SUM(C3:C5)</f>
         <v>38</v>
       </c>
-      <c r="D5">
-        <f t="shared" ref="D5:H5" si="0">SUM(D2:D4)</f>
+      <c r="D6">
+        <f t="shared" ref="D6:H6" si="0">SUM(D3:D5)</f>
         <v>13</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="2">
-        <f>B5/$H$5</f>
+    <row r="7" spans="1:8">
+      <c r="B7" s="2">
+        <f>B6/$H$6</f>
         <v>0.62307692307692308</v>
       </c>
-      <c r="C6" s="2">
-        <f t="shared" ref="C6:H6" si="1">C5/$H$5</f>
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:G7" si="1">C6/$H$6</f>
         <v>0.29230769230769232</v>
       </c>
-      <c r="D6" s="2">
-        <f>D5/$H$5</f>
+      <c r="D7" s="2">
+        <f>D6/$H$6</f>
         <v>0.1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>0.26923076923076922</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>8.461538461538462E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G7" s="2">
         <f t="shared" si="1"/>
         <v>3.0769230769230771E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" ht="60">
+      <c r="A10" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>147</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>0.62307692307692308</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>0.29230769230769232</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>0.1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>0.26923076923076922</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>8.461538461538462E-2</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G11" s="1">
         <v>3.0769230769230771E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hinzufügen Grafiken & Datenbereinigung
</commit_message>
<xml_diff>
--- a/data/auswertung-freitext-kategorien-open-access-meinung-30815.xlsx
+++ b/data/auswertung-freitext-kategorien-open-access-meinung-30815.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="154">
   <si>
     <t xml:space="preserve"> ich arbeite vorwiegend in präkeren arbeitsverhältnissen und investiere unbezahlte zeit in das verfassen meiner texte. wenn es die möglichkeit gibt, zumindest ein kleines honorar zu bekommen, dann bevorzuge ich das - ich muss ja irgendwie meine miete, mein essen, etc bezahlen.</t>
   </si>
@@ -484,14 +484,17 @@
     <t>a = Anerkennung, f = finanzielle Aspekte, q= Qualitäts Aspekte, s= strukturelle r=rechtliche, wf = wissenschaftsfreiheit</t>
   </si>
   <si>
-    <t>Frage: Bitte kommentieren Sie kurz Ihre Meinung zu der Forderung nach kostenfreiem Zugang zu allen wissenschaftlichen Publikationen (Open Access)</t>
+    <t>Frage: Bitte kommentieren Sie kurz Ihre Meinung zu der Forderung nach kostenfreiem Zugang zu allen wissenschaftlichen Publikationen (Open Access) - n=130</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,6 +518,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -533,7 +544,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="245">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -779,16 +790,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="245">
+  <cellStyles count="247">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -911,6 +926,7 @@
     <cellStyle name="Besuchter Link" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1033,6 +1049,7 @@
     <cellStyle name="Link" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1364,9 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1374,7 +1389,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1480,6 +1495,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
       <c r="B6">
         <f>SUM(B3:B5)</f>
         <v>81</v>
@@ -1534,6 +1552,7 @@
         <f t="shared" si="1"/>
         <v>3.0769230769230771E-2</v>
       </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="60">
       <c r="A10" t="s">
@@ -1601,7 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1859,7 +1878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>